<commit_message>
clear up stuff around Kurt Sievekings Cabinet
</commit_message>
<xml_diff>
--- a/inst/extdata/primeministers.xlsx
+++ b/inst/extdata/primeministers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\bldrt\bundeslaendeR\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\blcbadd\bundeslaendeR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907B2834-F8C1-4B0D-9DB4-9BEDFF4ACCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E20E431-1F4F-4270-B6A2-352AC6757E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -460,9 +460,6 @@
     <t>Brauer, Max</t>
   </si>
   <si>
-    <t>Sieveking</t>
-  </si>
-  <si>
     <t>Nevermann, Paul</t>
   </si>
   <si>
@@ -752,6 +749,9 @@
   </si>
   <si>
     <t>Rhein, Boris</t>
+  </si>
+  <si>
+    <t>Sieveking, Kurt</t>
   </si>
 </sst>
 </file>
@@ -1145,8 +1145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K371"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A325" workbookViewId="0">
-      <selection activeCell="A362" sqref="A362"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="I133" sqref="I133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4985,7 +4985,7 @@
         <v>47</v>
       </c>
       <c r="I132" t="s">
-        <v>146</v>
+        <v>243</v>
       </c>
       <c r="J132" t="s">
         <v>14</v>
@@ -5043,7 +5043,7 @@
         <v>9</v>
       </c>
       <c r="I134" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J134" t="s">
         <v>29</v>
@@ -5072,7 +5072,7 @@
         <v>9</v>
       </c>
       <c r="I135" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J135" t="s">
         <v>29</v>
@@ -5101,7 +5101,7 @@
         <v>9</v>
       </c>
       <c r="I136" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J136" t="s">
         <v>29</v>
@@ -5130,7 +5130,7 @@
         <v>29</v>
       </c>
       <c r="I137" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J137" t="s">
         <v>29</v>
@@ -5159,7 +5159,7 @@
         <v>9</v>
       </c>
       <c r="I138" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J138" t="s">
         <v>29</v>
@@ -5188,7 +5188,7 @@
         <v>9</v>
       </c>
       <c r="I139" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J139" t="s">
         <v>29</v>
@@ -5217,7 +5217,7 @@
         <v>9</v>
       </c>
       <c r="I140" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J140" t="s">
         <v>29</v>
@@ -5246,7 +5246,7 @@
         <v>9</v>
       </c>
       <c r="I141" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J141" t="s">
         <v>29</v>
@@ -5275,7 +5275,7 @@
         <v>29</v>
       </c>
       <c r="I142" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J142" t="s">
         <v>29</v>
@@ -5304,7 +5304,7 @@
         <v>29</v>
       </c>
       <c r="I143" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J143" t="s">
         <v>29</v>
@@ -5333,7 +5333,7 @@
         <v>29</v>
       </c>
       <c r="I144" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J144" t="s">
         <v>29</v>
@@ -5362,7 +5362,7 @@
         <v>29</v>
       </c>
       <c r="I145" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J145" t="s">
         <v>29</v>
@@ -5391,7 +5391,7 @@
         <v>29</v>
       </c>
       <c r="I146" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J146" t="s">
         <v>29</v>
@@ -5420,7 +5420,7 @@
         <v>9</v>
       </c>
       <c r="I147" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J147" t="s">
         <v>29</v>
@@ -5449,7 +5449,7 @@
         <v>9</v>
       </c>
       <c r="I148" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J148" t="s">
         <v>29</v>
@@ -5478,7 +5478,7 @@
         <v>29</v>
       </c>
       <c r="I149" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J149" t="s">
         <v>29</v>
@@ -5507,7 +5507,7 @@
         <v>29</v>
       </c>
       <c r="I150" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J150" t="s">
         <v>29</v>
@@ -5536,7 +5536,7 @@
         <v>30</v>
       </c>
       <c r="I151" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J151" t="s">
         <v>29</v>
@@ -5565,7 +5565,7 @@
         <v>48</v>
       </c>
       <c r="I152" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J152" t="s">
         <v>14</v>
@@ -5594,7 +5594,7 @@
         <v>14</v>
       </c>
       <c r="I153" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J153" t="s">
         <v>14</v>
@@ -5623,7 +5623,7 @@
         <v>49</v>
       </c>
       <c r="I154" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J154" t="s">
         <v>14</v>
@@ -5652,7 +5652,7 @@
         <v>49</v>
       </c>
       <c r="I155" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J155" t="s">
         <v>14</v>
@@ -5681,7 +5681,7 @@
         <v>14</v>
       </c>
       <c r="I156" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J156" t="s">
         <v>29</v>
@@ -5710,7 +5710,7 @@
         <v>29</v>
       </c>
       <c r="I157" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J157" t="s">
         <v>29</v>
@@ -5739,7 +5739,7 @@
         <v>30</v>
       </c>
       <c r="I158" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J158" t="s">
         <v>29</v>
@@ -5768,7 +5768,7 @@
         <v>30</v>
       </c>
       <c r="I159" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J159" t="s">
         <v>29</v>
@@ -5797,7 +5797,7 @@
         <v>30</v>
       </c>
       <c r="I160" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J160" t="s">
         <v>29</v>
@@ -5826,7 +5826,7 @@
         <v>28</v>
       </c>
       <c r="I161" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J161" t="s">
         <v>29</v>
@@ -5855,7 +5855,7 @@
         <v>29</v>
       </c>
       <c r="I162" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J162" t="s">
         <v>29</v>
@@ -5884,7 +5884,7 @@
         <v>51</v>
       </c>
       <c r="I163" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J163" t="s">
         <v>29</v>
@@ -5913,7 +5913,7 @@
         <v>51</v>
       </c>
       <c r="I164" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J164" t="s">
         <v>29</v>
@@ -5942,7 +5942,7 @@
         <v>52</v>
       </c>
       <c r="I165" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J165" t="s">
         <v>29</v>
@@ -5971,7 +5971,7 @@
         <v>29</v>
       </c>
       <c r="I166" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J166" t="s">
         <v>29</v>
@@ -6000,7 +6000,7 @@
         <v>29</v>
       </c>
       <c r="I167" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J167" t="s">
         <v>29</v>
@@ -6029,7 +6029,7 @@
         <v>9</v>
       </c>
       <c r="I168" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J168" t="s">
         <v>29</v>
@@ -6058,7 +6058,7 @@
         <v>9</v>
       </c>
       <c r="I169" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J169" t="s">
         <v>29</v>
@@ -6087,7 +6087,7 @@
         <v>9</v>
       </c>
       <c r="I170" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J170" t="s">
         <v>29</v>
@@ -6116,7 +6116,7 @@
         <v>9</v>
       </c>
       <c r="I171" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J171" t="s">
         <v>29</v>
@@ -6145,7 +6145,7 @@
         <v>29</v>
       </c>
       <c r="I172" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J172" t="s">
         <v>29</v>
@@ -6174,7 +6174,7 @@
         <v>29</v>
       </c>
       <c r="I173" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J173" t="s">
         <v>29</v>
@@ -6203,7 +6203,7 @@
         <v>30</v>
       </c>
       <c r="I174" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J174" t="s">
         <v>29</v>
@@ -6232,7 +6232,7 @@
         <v>29</v>
       </c>
       <c r="I175" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J175" t="s">
         <v>29</v>
@@ -6261,7 +6261,7 @@
         <v>12</v>
       </c>
       <c r="I176" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J176" t="s">
         <v>14</v>
@@ -6290,7 +6290,7 @@
         <v>30</v>
       </c>
       <c r="I177" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J177" t="s">
         <v>29</v>
@@ -6319,7 +6319,7 @@
         <v>30</v>
       </c>
       <c r="I178" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J178" t="s">
         <v>29</v>
@@ -6348,7 +6348,7 @@
         <v>12</v>
       </c>
       <c r="I179" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J179" t="s">
         <v>14</v>
@@ -6377,7 +6377,7 @@
         <v>14</v>
       </c>
       <c r="I180" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J180" t="s">
         <v>14</v>
@@ -6406,7 +6406,7 @@
         <v>14</v>
       </c>
       <c r="I181" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J181" t="s">
         <v>14</v>
@@ -6435,7 +6435,7 @@
         <v>12</v>
       </c>
       <c r="I182" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J182" t="s">
         <v>14</v>
@@ -6464,7 +6464,7 @@
         <v>12</v>
       </c>
       <c r="I183" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J183" t="s">
         <v>14</v>
@@ -6493,7 +6493,7 @@
         <v>49</v>
       </c>
       <c r="I184" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J184" t="s">
         <v>14</v>
@@ -6522,7 +6522,7 @@
         <v>49</v>
       </c>
       <c r="I185" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J185" t="s">
         <v>14</v>
@@ -6551,7 +6551,7 @@
         <v>49</v>
       </c>
       <c r="I186" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J186" t="s">
         <v>14</v>
@@ -6580,7 +6580,7 @@
         <v>12</v>
       </c>
       <c r="I187" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J187" t="s">
         <v>14</v>
@@ -6609,7 +6609,7 @@
         <v>12</v>
       </c>
       <c r="I188" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J188" t="s">
         <v>14</v>
@@ -6638,7 +6638,7 @@
         <v>13</v>
       </c>
       <c r="I189" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J189" t="s">
         <v>14</v>
@@ -6667,7 +6667,7 @@
         <v>31</v>
       </c>
       <c r="I190" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J190" t="s">
         <v>29</v>
@@ -6696,7 +6696,7 @@
         <v>31</v>
       </c>
       <c r="I191" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J191" t="s">
         <v>29</v>
@@ -6725,7 +6725,7 @@
         <v>28</v>
       </c>
       <c r="I192" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J192" t="s">
         <v>29</v>
@@ -6754,7 +6754,7 @@
         <v>28</v>
       </c>
       <c r="I193" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J193" t="s">
         <v>29</v>
@@ -6783,7 +6783,7 @@
         <v>28</v>
       </c>
       <c r="I194" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J194" t="s">
         <v>29</v>
@@ -6812,7 +6812,7 @@
         <v>28</v>
       </c>
       <c r="I195" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J195" t="s">
         <v>29</v>
@@ -6841,7 +6841,7 @@
         <v>28</v>
       </c>
       <c r="I196" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J196" t="s">
         <v>29</v>
@@ -6870,7 +6870,7 @@
         <v>31</v>
       </c>
       <c r="I197" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J197" t="s">
         <v>29</v>
@@ -6899,7 +6899,7 @@
         <v>55</v>
       </c>
       <c r="I198" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J198" t="s">
         <v>29</v>
@@ -6928,7 +6928,7 @@
         <v>56</v>
       </c>
       <c r="I199" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J199" t="s">
         <v>29</v>
@@ -6957,7 +6957,7 @@
         <v>57</v>
       </c>
       <c r="I200" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J200" t="s">
         <v>29</v>
@@ -6986,7 +6986,7 @@
         <v>58</v>
       </c>
       <c r="I201" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J201" t="s">
         <v>29</v>
@@ -7015,7 +7015,7 @@
         <v>59</v>
       </c>
       <c r="I202" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J202" t="s">
         <v>29</v>
@@ -7044,7 +7044,7 @@
         <v>51</v>
       </c>
       <c r="I203" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J203" t="s">
         <v>29</v>
@@ -7073,10 +7073,10 @@
         <v>60</v>
       </c>
       <c r="I204" t="s">
+        <v>172</v>
+      </c>
+      <c r="J204" t="s">
         <v>173</v>
-      </c>
-      <c r="J204" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.25">
@@ -7102,10 +7102,10 @@
         <v>61</v>
       </c>
       <c r="I205" t="s">
+        <v>172</v>
+      </c>
+      <c r="J205" t="s">
         <v>173</v>
-      </c>
-      <c r="J205" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.25">
@@ -7131,7 +7131,7 @@
         <v>62</v>
       </c>
       <c r="I206" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J206" t="s">
         <v>29</v>
@@ -7160,7 +7160,7 @@
         <v>62</v>
       </c>
       <c r="I207" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J207" t="s">
         <v>29</v>
@@ -7189,7 +7189,7 @@
         <v>9</v>
       </c>
       <c r="I208" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J208" t="s">
         <v>29</v>
@@ -7218,7 +7218,7 @@
         <v>28</v>
       </c>
       <c r="I209" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J209" t="s">
         <v>29</v>
@@ -7247,7 +7247,7 @@
         <v>28</v>
       </c>
       <c r="I210" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J210" t="s">
         <v>29</v>
@@ -7276,7 +7276,7 @@
         <v>29</v>
       </c>
       <c r="I211" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J211" t="s">
         <v>29</v>
@@ -7305,7 +7305,7 @@
         <v>9</v>
       </c>
       <c r="I212" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J212" t="s">
         <v>29</v>
@@ -7334,7 +7334,7 @@
         <v>43</v>
       </c>
       <c r="I213" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J213" t="s">
         <v>14</v>
@@ -7363,7 +7363,7 @@
         <v>14</v>
       </c>
       <c r="I214" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J214" t="s">
         <v>14</v>
@@ -7392,7 +7392,7 @@
         <v>12</v>
       </c>
       <c r="I215" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J215" t="s">
         <v>14</v>
@@ -7421,7 +7421,7 @@
         <v>14</v>
       </c>
       <c r="I216" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J216" t="s">
         <v>14</v>
@@ -7450,7 +7450,7 @@
         <v>14</v>
       </c>
       <c r="I217" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J217" t="s">
         <v>14</v>
@@ -7479,7 +7479,7 @@
         <v>12</v>
       </c>
       <c r="I218" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J218" t="s">
         <v>14</v>
@@ -7508,7 +7508,7 @@
         <v>30</v>
       </c>
       <c r="I219" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J219" t="s">
         <v>29</v>
@@ -7537,7 +7537,7 @@
         <v>29</v>
       </c>
       <c r="I220" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J220" t="s">
         <v>29</v>
@@ -7566,7 +7566,7 @@
         <v>29</v>
       </c>
       <c r="I221" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J221" t="s">
         <v>29</v>
@@ -7595,7 +7595,7 @@
         <v>29</v>
       </c>
       <c r="I222" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J222" t="s">
         <v>29</v>
@@ -7624,7 +7624,7 @@
         <v>29</v>
       </c>
       <c r="I223" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J223" t="s">
         <v>29</v>
@@ -7653,7 +7653,7 @@
         <v>12</v>
       </c>
       <c r="I224" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J224" t="s">
         <v>14</v>
@@ -7682,7 +7682,7 @@
         <v>12</v>
       </c>
       <c r="I225" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J225" t="s">
         <v>14</v>
@@ -7711,7 +7711,7 @@
         <v>12</v>
       </c>
       <c r="I226" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J226" t="s">
         <v>14</v>
@@ -7740,7 +7740,7 @@
         <v>30</v>
       </c>
       <c r="I227" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J227" t="s">
         <v>29</v>
@@ -7769,7 +7769,7 @@
         <v>28</v>
       </c>
       <c r="I228" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J228" t="s">
         <v>29</v>
@@ -7798,7 +7798,7 @@
         <v>64</v>
       </c>
       <c r="I229" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J229" t="s">
         <v>14</v>
@@ -7827,7 +7827,7 @@
         <v>65</v>
       </c>
       <c r="I230" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J230" t="s">
         <v>14</v>
@@ -7856,7 +7856,7 @@
         <v>14</v>
       </c>
       <c r="I231" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J231" t="s">
         <v>14</v>
@@ -7885,7 +7885,7 @@
         <v>66</v>
       </c>
       <c r="I232" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J232" t="s">
         <v>14</v>
@@ -7914,7 +7914,7 @@
         <v>67</v>
       </c>
       <c r="I233" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J233" t="s">
         <v>14</v>
@@ -7943,7 +7943,7 @@
         <v>68</v>
       </c>
       <c r="I234" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J234" t="s">
         <v>29</v>
@@ -7972,7 +7972,7 @@
         <v>14</v>
       </c>
       <c r="I235" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J235" t="s">
         <v>14</v>
@@ -8001,7 +8001,7 @@
         <v>12</v>
       </c>
       <c r="I236" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J236" t="s">
         <v>14</v>
@@ -8030,7 +8030,7 @@
         <v>12</v>
       </c>
       <c r="I237" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J237" t="s">
         <v>14</v>
@@ -8059,7 +8059,7 @@
         <v>14</v>
       </c>
       <c r="I238" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J238" t="s">
         <v>14</v>
@@ -8088,7 +8088,7 @@
         <v>9</v>
       </c>
       <c r="I239" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J239" t="s">
         <v>29</v>
@@ -8117,7 +8117,7 @@
         <v>9</v>
       </c>
       <c r="I240" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J240" t="s">
         <v>29</v>
@@ -8146,7 +8146,7 @@
         <v>9</v>
       </c>
       <c r="I241" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J241" t="s">
         <v>29</v>
@@ -8175,7 +8175,7 @@
         <v>9</v>
       </c>
       <c r="I242" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J242" t="s">
         <v>29</v>
@@ -8204,7 +8204,7 @@
         <v>29</v>
       </c>
       <c r="I243" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J243" t="s">
         <v>29</v>
@@ -8233,7 +8233,7 @@
         <v>29</v>
       </c>
       <c r="I244" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J244" t="s">
         <v>29</v>
@@ -8262,7 +8262,7 @@
         <v>29</v>
       </c>
       <c r="I245" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J245" t="s">
         <v>29</v>
@@ -8291,7 +8291,7 @@
         <v>30</v>
       </c>
       <c r="I246" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J246" t="s">
         <v>29</v>
@@ -8320,7 +8320,7 @@
         <v>30</v>
       </c>
       <c r="I247" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J247" t="s">
         <v>29</v>
@@ -8349,7 +8349,7 @@
         <v>30</v>
       </c>
       <c r="I248" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J248" t="s">
         <v>29</v>
@@ -8378,7 +8378,7 @@
         <v>30</v>
       </c>
       <c r="I249" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J249" t="s">
         <v>29</v>
@@ -8407,7 +8407,7 @@
         <v>12</v>
       </c>
       <c r="I250" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J250" t="s">
         <v>14</v>
@@ -8436,7 +8436,7 @@
         <v>30</v>
       </c>
       <c r="I251" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J251" t="s">
         <v>29</v>
@@ -8465,7 +8465,7 @@
         <v>30</v>
       </c>
       <c r="I252" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J252" t="s">
         <v>29</v>
@@ -8494,7 +8494,7 @@
         <v>12</v>
       </c>
       <c r="I253" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J253" t="s">
         <v>14</v>
@@ -8523,7 +8523,7 @@
         <v>12</v>
       </c>
       <c r="I254" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J254" t="s">
         <v>14</v>
@@ -8552,7 +8552,7 @@
         <v>49</v>
       </c>
       <c r="I255" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J255" t="s">
         <v>14</v>
@@ -8582,7 +8582,7 @@
         <v>70</v>
       </c>
       <c r="I256" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J256" t="s">
         <v>14</v>
@@ -8611,7 +8611,7 @@
         <v>13</v>
       </c>
       <c r="I257" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J257" t="s">
         <v>14</v>
@@ -8640,7 +8640,7 @@
         <v>14</v>
       </c>
       <c r="I258" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J258" t="s">
         <v>14</v>
@@ -8669,7 +8669,7 @@
         <v>13</v>
       </c>
       <c r="I259" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J259" t="s">
         <v>14</v>
@@ -8698,7 +8698,7 @@
         <v>12</v>
       </c>
       <c r="I260" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J260" t="s">
         <v>14</v>
@@ -8727,7 +8727,7 @@
         <v>12</v>
       </c>
       <c r="I261" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J261" t="s">
         <v>14</v>
@@ -8756,7 +8756,7 @@
         <v>12</v>
       </c>
       <c r="I262" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J262" t="s">
         <v>14</v>
@@ -8785,7 +8785,7 @@
         <v>12</v>
       </c>
       <c r="I263" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J263" t="s">
         <v>14</v>
@@ -8814,7 +8814,7 @@
         <v>12</v>
       </c>
       <c r="I264" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J264" t="s">
         <v>14</v>
@@ -8843,7 +8843,7 @@
         <v>12</v>
       </c>
       <c r="I265" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J265" t="s">
         <v>14</v>
@@ -8872,7 +8872,7 @@
         <v>14</v>
       </c>
       <c r="I266" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J266" t="s">
         <v>14</v>
@@ -8901,7 +8901,7 @@
         <v>14</v>
       </c>
       <c r="I267" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J267" t="s">
         <v>14</v>
@@ -8930,7 +8930,7 @@
         <v>14</v>
       </c>
       <c r="I268" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J268" t="s">
         <v>14</v>
@@ -8959,7 +8959,7 @@
         <v>14</v>
       </c>
       <c r="I269" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J269" t="s">
         <v>14</v>
@@ -8988,7 +8988,7 @@
         <v>14</v>
       </c>
       <c r="I270" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J270" t="s">
         <v>14</v>
@@ -9017,7 +9017,7 @@
         <v>12</v>
       </c>
       <c r="I271" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J271" t="s">
         <v>14</v>
@@ -9046,7 +9046,7 @@
         <v>12</v>
       </c>
       <c r="I272" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J272" t="s">
         <v>14</v>
@@ -9075,7 +9075,7 @@
         <v>9</v>
       </c>
       <c r="I273" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J273" t="s">
         <v>29</v>
@@ -9104,7 +9104,7 @@
         <v>9</v>
       </c>
       <c r="I274" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J274" t="s">
         <v>29</v>
@@ -9133,7 +9133,7 @@
         <v>9</v>
       </c>
       <c r="I275" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J275" t="s">
         <v>29</v>
@@ -9162,7 +9162,7 @@
         <v>28</v>
       </c>
       <c r="I276" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J276" t="s">
         <v>29</v>
@@ -9191,7 +9191,7 @@
         <v>29</v>
       </c>
       <c r="I277" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J277" t="s">
         <v>29</v>
@@ -9220,7 +9220,7 @@
         <v>30</v>
       </c>
       <c r="I278" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J278" t="s">
         <v>29</v>
@@ -9249,7 +9249,7 @@
         <v>30</v>
       </c>
       <c r="I279" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J279" t="s">
         <v>29</v>
@@ -9278,7 +9278,7 @@
         <v>35</v>
       </c>
       <c r="I280" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J280" t="s">
         <v>29</v>
@@ -9307,7 +9307,7 @@
         <v>40</v>
       </c>
       <c r="I281" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J281" t="s">
         <v>29</v>
@@ -9336,7 +9336,7 @@
         <v>72</v>
       </c>
       <c r="I282" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J282" t="s">
         <v>73</v>
@@ -9365,7 +9365,7 @@
         <v>73</v>
       </c>
       <c r="I283" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J283" t="s">
         <v>73</v>
@@ -9394,7 +9394,7 @@
         <v>72</v>
       </c>
       <c r="I284" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J284" t="s">
         <v>73</v>
@@ -9423,7 +9423,7 @@
         <v>73</v>
       </c>
       <c r="I285" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J285" t="s">
         <v>73</v>
@@ -9455,10 +9455,10 @@
         <v>75</v>
       </c>
       <c r="I286" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J286" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="287" spans="1:10" x14ac:dyDescent="0.25">
@@ -9484,7 +9484,7 @@
         <v>76</v>
       </c>
       <c r="I287" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J287" t="s">
         <v>14</v>
@@ -9513,7 +9513,7 @@
         <v>13</v>
       </c>
       <c r="I288" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J288" t="s">
         <v>14</v>
@@ -9542,7 +9542,7 @@
         <v>76</v>
       </c>
       <c r="I289" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J289" t="s">
         <v>14</v>
@@ -9571,7 +9571,7 @@
         <v>77</v>
       </c>
       <c r="I290" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J290" t="s">
         <v>14</v>
@@ -9600,7 +9600,7 @@
         <v>13</v>
       </c>
       <c r="I291" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J291" t="s">
         <v>14</v>
@@ -9629,7 +9629,7 @@
         <v>12</v>
       </c>
       <c r="I292" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J292" t="s">
         <v>14</v>
@@ -9658,7 +9658,7 @@
         <v>12</v>
       </c>
       <c r="I293" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J293" t="s">
         <v>14</v>
@@ -9687,7 +9687,7 @@
         <v>14</v>
       </c>
       <c r="I294" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J294" t="s">
         <v>14</v>
@@ -9716,7 +9716,7 @@
         <v>14</v>
       </c>
       <c r="I295" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J295" t="s">
         <v>14</v>
@@ -9745,7 +9745,7 @@
         <v>12</v>
       </c>
       <c r="I296" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J296" t="s">
         <v>14</v>
@@ -9774,7 +9774,7 @@
         <v>12</v>
       </c>
       <c r="I297" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J297" t="s">
         <v>14</v>
@@ -9803,7 +9803,7 @@
         <v>12</v>
       </c>
       <c r="I298" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J298" t="s">
         <v>14</v>
@@ -9832,7 +9832,7 @@
         <v>29</v>
       </c>
       <c r="I299" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J299" t="s">
         <v>29</v>
@@ -9861,7 +9861,7 @@
         <v>29</v>
       </c>
       <c r="I300" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J300" t="s">
         <v>29</v>
@@ -9890,7 +9890,7 @@
         <v>29</v>
       </c>
       <c r="I301" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J301" t="s">
         <v>29</v>
@@ -9919,7 +9919,7 @@
         <v>29</v>
       </c>
       <c r="I302" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J302" t="s">
         <v>29</v>
@@ -9948,7 +9948,7 @@
         <v>14</v>
       </c>
       <c r="I303" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J303" t="s">
         <v>14</v>
@@ -9977,7 +9977,7 @@
         <v>14</v>
       </c>
       <c r="I304" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J304" t="s">
         <v>14</v>
@@ -10006,7 +10006,7 @@
         <v>78</v>
       </c>
       <c r="I305" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J305" t="s">
         <v>14</v>
@@ -10035,7 +10035,7 @@
         <v>78</v>
       </c>
       <c r="I306" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J306" t="s">
         <v>14</v>
@@ -10064,7 +10064,7 @@
         <v>14</v>
       </c>
       <c r="I307" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J307" t="s">
         <v>14</v>
@@ -10093,7 +10093,7 @@
         <v>13</v>
       </c>
       <c r="I308" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J308" t="s">
         <v>14</v>
@@ -10122,7 +10122,7 @@
         <v>13</v>
       </c>
       <c r="I309" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J309" t="s">
         <v>14</v>
@@ -10151,7 +10151,7 @@
         <v>13</v>
       </c>
       <c r="I310" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J310" t="s">
         <v>14</v>
@@ -10180,7 +10180,7 @@
         <v>29</v>
       </c>
       <c r="I311" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J311" t="s">
         <v>29</v>
@@ -10209,7 +10209,7 @@
         <v>14</v>
       </c>
       <c r="I312" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J312" t="s">
         <v>14</v>
@@ -10238,7 +10238,7 @@
         <v>14</v>
       </c>
       <c r="I313" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J313" t="s">
         <v>14</v>
@@ -10267,7 +10267,7 @@
         <v>14</v>
       </c>
       <c r="I314" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J314" t="s">
         <v>14</v>
@@ -10296,7 +10296,7 @@
         <v>14</v>
       </c>
       <c r="I315" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J315" t="s">
         <v>14</v>
@@ -10325,7 +10325,7 @@
         <v>13</v>
       </c>
       <c r="I316" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J316" t="s">
         <v>14</v>
@@ -10354,7 +10354,7 @@
         <v>13</v>
       </c>
       <c r="I317" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J317" t="s">
         <v>14</v>
@@ -10383,7 +10383,7 @@
         <v>12</v>
       </c>
       <c r="I318" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J318" t="s">
         <v>14</v>
@@ -10412,7 +10412,7 @@
         <v>13</v>
       </c>
       <c r="I319" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J319" t="s">
         <v>14</v>
@@ -10441,7 +10441,7 @@
         <v>13</v>
       </c>
       <c r="I320" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J320" t="s">
         <v>14</v>
@@ -10470,7 +10470,7 @@
         <v>80</v>
       </c>
       <c r="I321" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J321" t="s">
         <v>14</v>
@@ -10499,7 +10499,7 @@
         <v>12</v>
       </c>
       <c r="I322" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J322" t="s">
         <v>14</v>
@@ -10528,7 +10528,7 @@
         <v>12</v>
       </c>
       <c r="I323" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J323" t="s">
         <v>14</v>
@@ -10557,7 +10557,7 @@
         <v>12</v>
       </c>
       <c r="I324" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J324" t="s">
         <v>14</v>
@@ -10586,7 +10586,7 @@
         <v>30</v>
       </c>
       <c r="I325" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J325" t="s">
         <v>29</v>
@@ -10615,7 +10615,7 @@
         <v>29</v>
       </c>
       <c r="I326" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J326" t="s">
         <v>29</v>
@@ -10644,7 +10644,7 @@
         <v>12</v>
       </c>
       <c r="I327" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J327" t="s">
         <v>14</v>
@@ -10673,7 +10673,7 @@
         <v>13</v>
       </c>
       <c r="I328" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J328" t="s">
         <v>14</v>
@@ -10702,7 +10702,7 @@
         <v>13</v>
       </c>
       <c r="I329" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J329" t="s">
         <v>14</v>
@@ -10731,7 +10731,7 @@
         <v>82</v>
       </c>
       <c r="I330" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J330" t="s">
         <v>14</v>
@@ -10760,7 +10760,7 @@
         <v>43</v>
       </c>
       <c r="I331" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J331" t="s">
         <v>14</v>
@@ -10789,7 +10789,7 @@
         <v>29</v>
       </c>
       <c r="I332" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J332" t="s">
         <v>29</v>
@@ -10818,7 +10818,7 @@
         <v>29</v>
       </c>
       <c r="I333" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J333" t="s">
         <v>29</v>
@@ -10847,7 +10847,7 @@
         <v>84</v>
       </c>
       <c r="I334" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J334" t="s">
         <v>14</v>
@@ -10876,7 +10876,7 @@
         <v>12</v>
       </c>
       <c r="I335" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J335" t="s">
         <v>14</v>
@@ -10905,7 +10905,7 @@
         <v>84</v>
       </c>
       <c r="I336" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J336" t="s">
         <v>14</v>
@@ -10934,7 +10934,7 @@
         <v>85</v>
       </c>
       <c r="I337" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J337" t="s">
         <v>14</v>
@@ -10963,7 +10963,7 @@
         <v>86</v>
       </c>
       <c r="I338" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J338" t="s">
         <v>14</v>
@@ -10992,7 +10992,7 @@
         <v>87</v>
       </c>
       <c r="I339" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J339" t="s">
         <v>14</v>
@@ -11021,7 +11021,7 @@
         <v>12</v>
       </c>
       <c r="I340" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J340" t="s">
         <v>14</v>
@@ -11050,7 +11050,7 @@
         <v>14</v>
       </c>
       <c r="I341" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J341" t="s">
         <v>14</v>
@@ -11079,7 +11079,7 @@
         <v>12</v>
       </c>
       <c r="I342" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J342" t="s">
         <v>14</v>
@@ -11108,7 +11108,7 @@
         <v>12</v>
       </c>
       <c r="I343" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J343" t="s">
         <v>14</v>
@@ -11137,7 +11137,7 @@
         <v>14</v>
       </c>
       <c r="I344" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J344" t="s">
         <v>14</v>
@@ -11166,7 +11166,7 @@
         <v>14</v>
       </c>
       <c r="I345" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J345" t="s">
         <v>14</v>
@@ -11195,7 +11195,7 @@
         <v>14</v>
       </c>
       <c r="I346" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J346" t="s">
         <v>14</v>
@@ -11224,7 +11224,7 @@
         <v>14</v>
       </c>
       <c r="I347" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J347" t="s">
         <v>14</v>
@@ -11253,7 +11253,7 @@
         <v>14</v>
       </c>
       <c r="I348" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J348" t="s">
         <v>14</v>
@@ -11282,7 +11282,7 @@
         <v>14</v>
       </c>
       <c r="I349" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J349" t="s">
         <v>14</v>
@@ -11311,7 +11311,7 @@
         <v>14</v>
       </c>
       <c r="I350" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J350" t="s">
         <v>14</v>
@@ -11340,7 +11340,7 @@
         <v>14</v>
       </c>
       <c r="I351" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J351" t="s">
         <v>14</v>
@@ -11369,7 +11369,7 @@
         <v>29</v>
       </c>
       <c r="I352" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J352" t="s">
         <v>29</v>
@@ -11398,7 +11398,7 @@
         <v>29</v>
       </c>
       <c r="I353" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J353" t="s">
         <v>29</v>
@@ -11427,7 +11427,7 @@
         <v>29</v>
       </c>
       <c r="I354" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J354" t="s">
         <v>29</v>
@@ -11456,7 +11456,7 @@
         <v>30</v>
       </c>
       <c r="I355" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J355" t="s">
         <v>29</v>
@@ -11485,7 +11485,7 @@
         <v>30</v>
       </c>
       <c r="I356" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J356" t="s">
         <v>29</v>
@@ -11514,7 +11514,7 @@
         <v>13</v>
       </c>
       <c r="I357" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J357" t="s">
         <v>14</v>
@@ -11543,7 +11543,7 @@
         <v>12</v>
       </c>
       <c r="I358" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J358" t="s">
         <v>14</v>
@@ -11572,7 +11572,7 @@
         <v>88</v>
       </c>
       <c r="I359" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J359" t="s">
         <v>29</v>
@@ -11601,7 +11601,7 @@
         <v>89</v>
       </c>
       <c r="I360" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J360" t="s">
         <v>14</v>
@@ -11630,7 +11630,7 @@
         <v>49</v>
       </c>
       <c r="I361" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J361" t="s">
         <v>14</v>
@@ -11659,7 +11659,7 @@
         <v>12</v>
       </c>
       <c r="I362" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J362" t="s">
         <v>14</v>
@@ -11688,7 +11688,7 @@
         <v>12</v>
       </c>
       <c r="I363" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J363" t="s">
         <v>14</v>
@@ -11717,7 +11717,7 @@
         <v>13</v>
       </c>
       <c r="I364" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J364" t="s">
         <v>14</v>
@@ -11746,7 +11746,7 @@
         <v>14</v>
       </c>
       <c r="I365" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J365" t="s">
         <v>14</v>
@@ -11775,7 +11775,7 @@
         <v>14</v>
       </c>
       <c r="I366" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J366" t="s">
         <v>14</v>
@@ -11804,7 +11804,7 @@
         <v>14</v>
       </c>
       <c r="I367" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J367" t="s">
         <v>14</v>
@@ -11833,7 +11833,7 @@
         <v>13</v>
       </c>
       <c r="I368" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J368" t="s">
         <v>14</v>
@@ -11862,7 +11862,7 @@
         <v>91</v>
       </c>
       <c r="I369" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J369" t="s">
         <v>133</v>
@@ -11891,7 +11891,7 @@
         <v>92</v>
       </c>
       <c r="I370" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J370" t="s">
         <v>92</v>
@@ -11920,7 +11920,7 @@
         <v>91</v>
       </c>
       <c r="I371" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J371" t="s">
         <v>133</v>

</xml_diff>